<commit_message>
updated results with new values
</commit_message>
<xml_diff>
--- a/results/first_implementation.xlsx
+++ b/results/first_implementation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://her169626-my.sharepoint.com/personal/f_kretke_otto-hahn-gymnasium_de/Documents/Schule/Facharbeit/facharbeit/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="11_AD4DB114E441178AC67DF4526E55E246693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CD9EEFB-8C81-4C0C-8344-5EB9DB49F2E1}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="11_AD4DB114E441178AC67DF4526E55E246693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF37DD99-A29F-4A2C-BFA2-E5D0E7C32B5F}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="1335" windowWidth="31875" windowHeight="17145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -346,31 +346,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>6340</c:v>
+                  <c:v>6900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12870</c:v>
+                  <c:v>13720</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27250</c:v>
+                  <c:v>28380</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62470</c:v>
+                  <c:v>69960</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>136330</c:v>
+                  <c:v>154600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>333810</c:v>
+                  <c:v>432150</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>702540</c:v>
+                  <c:v>1347540</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2033710</c:v>
+                  <c:v>4532630</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3954970</c:v>
+                  <c:v>16446350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -556,31 +556,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>8070</c:v>
+                  <c:v>8160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17680</c:v>
+                  <c:v>18020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46720</c:v>
+                  <c:v>39220</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90340</c:v>
+                  <c:v>84860</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>192170</c:v>
+                  <c:v>180460</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>410520</c:v>
+                  <c:v>378480</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>891630</c:v>
+                  <c:v>757480</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1855790</c:v>
+                  <c:v>1508130</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4008190</c:v>
+                  <c:v>3012890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -766,31 +766,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>71740</c:v>
+                  <c:v>75050</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>284590</c:v>
+                  <c:v>291030</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1178390</c:v>
+                  <c:v>1165580</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4623850</c:v>
+                  <c:v>4668220</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18689580</c:v>
+                  <c:v>18541010</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74689470</c:v>
+                  <c:v>74027310</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>301373550</c:v>
+                  <c:v>294371060</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1205930460</c:v>
+                  <c:v>1183581160</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4842500730</c:v>
+                  <c:v>4725895550</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1368,31 +1368,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>6340</c:v>
+                  <c:v>6900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12870</c:v>
+                  <c:v>13720</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27250</c:v>
+                  <c:v>28380</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62470</c:v>
+                  <c:v>69960</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>136330</c:v>
+                  <c:v>154600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>333810</c:v>
+                  <c:v>432150</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>702540</c:v>
+                  <c:v>1347540</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2033710</c:v>
+                  <c:v>4532630</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3954970</c:v>
+                  <c:v>16446350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,31 +1578,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>8070</c:v>
+                  <c:v>8160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17680</c:v>
+                  <c:v>18020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46720</c:v>
+                  <c:v>39220</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90340</c:v>
+                  <c:v>84860</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>192170</c:v>
+                  <c:v>180460</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>410520</c:v>
+                  <c:v>378480</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>891630</c:v>
+                  <c:v>757480</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1855790</c:v>
+                  <c:v>1508130</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4008190</c:v>
+                  <c:v>3012890</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3115,10 +3115,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3385,7 +3381,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,31 +3461,31 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>6340</v>
+        <v>6900</v>
       </c>
       <c r="C3">
-        <v>12870</v>
+        <v>13720</v>
       </c>
       <c r="D3">
-        <v>27250</v>
+        <v>28380</v>
       </c>
       <c r="E3">
-        <v>62470</v>
+        <v>69960</v>
       </c>
       <c r="F3">
-        <v>136330</v>
+        <v>154600</v>
       </c>
       <c r="G3">
-        <v>333810</v>
+        <v>432150</v>
       </c>
       <c r="H3">
-        <v>702540</v>
+        <v>1347540</v>
       </c>
       <c r="I3">
-        <v>2033710</v>
+        <v>4532630</v>
       </c>
       <c r="J3">
-        <v>3954970</v>
+        <v>16446350</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3529,31 +3525,31 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>8070</v>
+        <v>8160</v>
       </c>
       <c r="C5">
-        <v>17680</v>
+        <v>18020</v>
       </c>
       <c r="D5">
-        <v>46720</v>
+        <v>39220</v>
       </c>
       <c r="E5">
-        <v>90340</v>
+        <v>84860</v>
       </c>
       <c r="F5">
-        <v>192170</v>
+        <v>180460</v>
       </c>
       <c r="G5">
-        <v>410520</v>
+        <v>378480</v>
       </c>
       <c r="H5">
-        <v>891630</v>
+        <v>757480</v>
       </c>
       <c r="I5">
-        <v>1855790</v>
+        <v>1508130</v>
       </c>
       <c r="J5">
-        <v>4008190</v>
+        <v>3012890</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3593,31 +3589,31 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>71740</v>
+        <v>75050</v>
       </c>
       <c r="C7">
-        <v>284590</v>
+        <v>291030</v>
       </c>
       <c r="D7">
-        <v>1178390</v>
+        <v>1165580</v>
       </c>
       <c r="E7">
-        <v>4623850</v>
+        <v>4668220</v>
       </c>
       <c r="F7">
-        <v>18689580</v>
+        <v>18541010</v>
       </c>
       <c r="G7">
-        <v>74689470</v>
+        <v>74027310</v>
       </c>
       <c r="H7">
-        <v>301373550</v>
+        <v>294371060</v>
       </c>
       <c r="I7">
-        <v>1205930460</v>
+        <v>1183581160</v>
       </c>
       <c r="J7">
-        <v>4842500730</v>
+        <v>4725895550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>